<commit_message>
Updated AUS model - 2025-08-07 15:41
</commit_message>
<xml_diff>
--- a/VerveStacks_AUS/vt_vervestacks_AUS_v1.xlsx
+++ b/VerveStacks_AUS/vt_vervestacks_AUS_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_AUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B621DD8B-0AA5-4772-AE62-2AD6492F8A25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{28FECEA2-EC9A-4F0D-BB88-8DA944E7E8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{6DBEF337-55C3-46B3-895A-B6BF79CEC6B8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{CFBCE5F7-36ED-4202-B405-620AAF314998}"/>
   </bookViews>
   <sheets>
     <sheet name="weo_pg" sheetId="3" r:id="rId1"/>
@@ -952,7 +952,7 @@
     <t>ep_wind_onshore_G100000927837</t>
   </si>
   <si>
-    <t>VERVESTACKS: the open USE platform. Powered by data | Guided by intuition | Built with AI.</t>
+    <t>VERVESTACKS - the open USE platform · Powered by data · Shaped by intuition · Accelerated with AI</t>
   </si>
   <si>
     <t>~fi_process</t>
@@ -2754,7 +2754,7 @@
     </font>
     <font>
       <b/>
-      <sz val="7"/>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -3184,7 +3184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04AB302-1C9E-4A0E-9863-2211345D1676}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77890C6B-4BE1-42F9-B5A4-6E3D2BCB979A}">
   <dimension ref="A1:Q107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6172,7 +6172,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6187100-F1D8-4D00-8558-4DBE97657F72}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56F23522-6F04-49AD-B120-8E5FC94EB833}">
   <dimension ref="A1:U140"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -13963,7 +13963,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDDF59DC-9C60-4556-97BE-A1F8429CBB5B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555E2EC2-751A-46CF-B029-8CAFF4B33B88}">
   <dimension ref="A1:T354"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>